<commit_message>
Added three students to our mailing list
</commit_message>
<xml_diff>
--- a/Student Names.xlsx
+++ b/Student Names.xlsx
@@ -16,6 +16,47 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Surname</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>Keith</t>
+  </si>
+  <si>
+    <t>Manny</t>
+  </si>
+  <si>
+    <t>Yellow</t>
+  </si>
+  <si>
+    <t>Mary</t>
+  </si>
+  <si>
+    <t>Johnson</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>Jonathan</t>
+  </si>
+  <si>
+    <t>Fielding</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -37,7 +78,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -45,18 +86,190 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -331,12 +544,79 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="35" customWidth="1"/>
+    <col min="3" max="3" width="32" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="6"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="6"/>
+    </row>
+    <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="7"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="9"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>